<commit_message>
Update on 20250522 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -11,12 +11,17 @@
     <sheet name="卫视" sheetId="1" r:id="rId2"/>
     <sheet name="中教,CHC和央视付费" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">上海!$A$1:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">卫视!$A$1:$D$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'中教,CHC和央视付费'!$A$1:$D$23</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
   <si>
     <t>东方卫视</t>
   </si>
@@ -138,10 +143,6 @@
     <t>浙江卫视</t>
   </si>
   <si>
-    <t>网络</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>高清</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,10 +155,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OCN机顶盒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陕西农林卫视</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -382,6 +379,102 @@
   </si>
   <si>
     <t>CHC影迷电影</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络高清源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPTV源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,BPTV源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,BPTV源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPTV源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>BPTV源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒店源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该颜色字体为为不稳定源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香港卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方有线机顶盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络标清源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,7 +482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +512,21 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -481,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -491,6 +599,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -798,27 +908,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -827,287 +936,288 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="3"/>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D25"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1115,513 +1225,610 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="F2" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C6" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C14" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+        <v>113</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C27" s="1"/>
+      <c r="D27" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C30" s="1"/>
+      <c r="D30" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C34" s="1"/>
+      <c r="D34" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C37" s="1"/>
+      <c r="D37" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="C43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="B46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1636,299 +1843,299 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D23"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250522 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="129">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1227,7 +1227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1708,7 +1710,9 @@
       <c r="B37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="D37" s="10" t="s">
         <v>124</v>
       </c>
@@ -1720,7 +1724,9 @@
       <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="D38" s="8" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250525 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="129">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1138,20 +1138,24 @@
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -1200,10 +1204,12 @@
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250530 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="132">
   <si>
     <t>东方卫视</t>
   </si>
@@ -386,18 +386,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BPTV源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,BPTV源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,BPTV源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源</t>
   </si>
   <si>
@@ -405,10 +393,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BPTV源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -429,20 +413,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BPTV源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BPTV源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源,咪咕源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>酒店源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该颜色字体为为不稳定源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香港卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方有线机顶盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络标清源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+  </si>
+  <si>
+    <t>咪咕源</t>
+  </si>
+  <si>
+    <t>酒店源</t>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>BPTV源,</t>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>官方源,</t>
     </r>
     <r>
       <rPr>
@@ -458,23 +474,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该颜色字体为为不稳定源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>香港卫视</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东方有线机顶盒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络标清源</t>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -482,7 +498,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,6 +543,13 @@
       <color theme="9" tint="-0.249977111117893"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -906,14 +929,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -931,7 +954,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +970,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -965,7 +988,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -983,7 +1006,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
@@ -993,7 +1016,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1007,7 +1030,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1021,7 +1044,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1035,7 +1058,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>71</v>
       </c>
@@ -1049,7 +1072,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>73</v>
       </c>
@@ -1059,7 +1082,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1069,7 +1092,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1079,7 +1102,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -1091,7 +1114,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1103,7 +1126,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
@@ -1113,7 +1136,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1125,7 +1148,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1134,7 +1157,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1146,7 +1169,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1158,7 +1181,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1168,7 +1191,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1180,7 +1203,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1190,7 +1213,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -1200,7 +1223,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -1212,7 +1235,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -1233,11 +1256,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -1245,24 +1266,24 @@
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,14 +1291,14 @@
         <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1285,11 +1306,11 @@
         <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1297,11 +1318,11 @@
         <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1309,25 +1330,21 @@
         <v>41</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+        <v>111</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1336,10 +1353,10 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1347,11 +1364,11 @@
         <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1360,10 +1377,10 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1371,11 +1388,11 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1383,27 +1400,23 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1411,11 +1424,13 @@
         <v>41</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+        <v>127</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1423,11 +1438,11 @@
         <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1435,13 +1450,13 @@
         <v>40</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1449,13 +1464,13 @@
         <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1463,11 +1478,11 @@
         <v>40</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1475,23 +1490,21 @@
         <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1499,11 +1512,13 @@
         <v>40</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1511,11 +1526,11 @@
         <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1523,23 +1538,21 @@
         <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1547,13 +1560,13 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1561,13 +1574,11 @@
         <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1575,13 +1586,11 @@
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1590,10 +1599,10 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1602,10 +1611,10 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1613,13 +1622,13 @@
         <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1627,11 +1636,9 @@
         <v>42</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1639,25 +1646,23 @@
         <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -1665,13 +1670,11 @@
         <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -1680,10 +1683,10 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1691,25 +1694,23 @@
         <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+        <v>113</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1720,10 +1721,10 @@
         <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1733,23 +1734,19 @@
       <c r="C38" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C39" s="8"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1757,11 +1754,11 @@
         <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
@@ -1769,25 +1766,23 @@
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
@@ -1795,13 +1790,11 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -1809,11 +1802,11 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -1821,13 +1814,11 @@
         <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
@@ -1835,7 +1826,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="D46" s="1"/>
     </row>
@@ -1853,14 +1844,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -1878,7 +1869,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
@@ -1896,7 +1887,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -1910,7 +1901,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -1924,7 +1915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>88</v>
       </c>
@@ -1934,7 +1925,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -1946,7 +1937,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>90</v>
       </c>
@@ -1956,7 +1947,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>91</v>
       </c>
@@ -1970,7 +1961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
@@ -1984,7 +1975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>93</v>
       </c>
@@ -1998,7 +1989,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>94</v>
       </c>
@@ -2012,7 +2003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
@@ -2022,7 +2013,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>96</v>
       </c>
@@ -2032,7 +2023,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>97</v>
       </c>
@@ -2044,7 +2035,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -2054,7 +2045,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>99</v>
       </c>
@@ -2064,7 +2055,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2074,7 +2065,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2084,7 +2075,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2094,7 +2085,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
@@ -2104,7 +2095,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" s="8" t="s">
         <v>107</v>
       </c>
@@ -2118,7 +2109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="8" t="s">
         <v>105</v>
       </c>
@@ -2132,7 +2123,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="8" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250601 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="135">
   <si>
     <t>东方卫视</t>
   </si>
@@ -401,53 +401,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒店源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该颜色字体为为不稳定源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香港卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方有线机顶盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络标清源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+  </si>
+  <si>
     <t>咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该颜色字体为为不稳定源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>香港卫视</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东方有线机顶盒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络标清源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
-  </si>
-  <si>
-    <t>咪咕源</t>
-  </si>
-  <si>
-    <t>酒店源</t>
-  </si>
-  <si>
-    <t>官方源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -474,23 +462,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,咪咕源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>官方源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源</t>
+    <t>官方源,NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1271,13 +1283,13 @@
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>77</v>
@@ -1291,11 +1303,11 @@
         <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1306,7 +1318,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1318,7 +1330,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -1341,7 +1353,9 @@
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:6">
@@ -1353,7 +1367,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1364,7 +1378,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1375,9 +1389,11 @@
       <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="D9" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1388,7 +1404,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1400,7 +1416,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1411,9 +1427,11 @@
       <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="D12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1424,7 +1442,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>75</v>
@@ -1438,7 +1456,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1450,7 +1468,7 @@
         <v>40</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>110</v>
@@ -1464,10 +1482,10 @@
         <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1478,7 +1496,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1490,7 +1508,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1501,7 +1519,9 @@
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4">
@@ -1515,7 +1535,7 @@
         <v>129</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1526,7 +1546,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1538,7 +1558,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1549,7 +1569,9 @@
       <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4">
@@ -1560,10 +1582,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1574,7 +1596,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="D25" s="8"/>
     </row>
@@ -1586,7 +1608,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D26" s="8"/>
     </row>
@@ -1599,7 +1621,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1609,9 +1631,11 @@
       <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="D28" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1625,7 +1649,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1649,7 +1673,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1659,7 +1683,9 @@
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4">
@@ -1670,7 +1696,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D33" s="8"/>
     </row>
@@ -1683,7 +1709,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1694,7 +1720,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>70</v>
@@ -1707,7 +1733,9 @@
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4">
@@ -1721,7 +1749,7 @@
         <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1732,7 +1760,7 @@
         <v>40</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="D38" s="8"/>
     </row>
@@ -1743,7 +1771,9 @@
       <c r="B39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4">
@@ -1766,13 +1796,13 @@
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>42</v>
@@ -1790,7 +1820,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D43" s="8"/>
     </row>
@@ -1814,7 +1844,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D45" s="8"/>
     </row>
@@ -1826,7 +1856,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D46" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250604 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="175">
   <si>
     <t>东方卫视</t>
   </si>
@@ -407,10 +407,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官方源,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>该颜色字体为为不稳定源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -427,16 +423,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官方源,咪咕源</t>
-  </si>
-  <si>
     <t>咪咕源</t>
   </si>
   <si>
-    <t>咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源,咪咕源,NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -453,18 +442,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕源,NPTV源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源,NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官方源,咪咕源,NPTV源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -487,14 +468,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官方源,咪咕源,NPTV源,安徽联通酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官方源,咪咕源,NPTV源,安徽联通酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源,咪咕源,安徽联通酒店源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -613,6 +586,128 @@
   </si>
   <si>
     <t>CCTV-4欧洲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源,安徽联通酒店源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>官方源,NPTV源,安徽联通酒店源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>NPTV源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>NPTV源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>官方源,NPTV源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>官方源,NPTV源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>NPTV源,安徽联通酒店源,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上海电信酒店源</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,7 +715,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -664,6 +759,21 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -726,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -738,6 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1065,7 +1176,7 @@
         <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>77</v>
@@ -1074,19 +1185,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
@@ -1095,52 +1206,52 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1151,7 +1262,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
@@ -1162,177 +1273,177 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="8"/>
@@ -1340,13 +1451,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
@@ -1362,7 +1473,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1377,7 +1488,7 @@
         <v>76</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1392,84 +1503,84 @@
         <v>76</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="1"/>
@@ -1493,7 +1604,7 @@
         <v>76</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1514,10 +1625,10 @@
         <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>76</v>
@@ -1529,10 +1640,10 @@
         <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>76</v>
@@ -1544,10 +1655,10 @@
         <v>93</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>76</v>
@@ -1559,10 +1670,10 @@
         <v>94</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>76</v>
@@ -1599,7 +1710,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2017,7 +2128,7 @@
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2027,13 +2138,13 @@
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>77</v>
@@ -2047,11 +2158,11 @@
         <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="F2" s="9" t="s">
-        <v>115</v>
+      <c r="F2" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2074,7 +2185,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2098,7 +2209,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2113,6 +2224,7 @@
       <c r="D7" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
@@ -2122,7 +2234,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2134,10 +2246,10 @@
         <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2148,7 +2260,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2160,7 +2272,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2172,10 +2284,10 @@
         <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2186,11 +2298,9 @@
         <v>41</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
@@ -2200,7 +2310,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2212,7 +2322,7 @@
         <v>40</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>110</v>
@@ -2226,11 +2336,9 @@
         <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
@@ -2240,7 +2348,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2252,7 +2360,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2264,7 +2372,7 @@
         <v>40</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2276,11 +2384,9 @@
         <v>40</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
@@ -2290,7 +2396,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2302,7 +2408,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2314,7 +2420,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2326,10 +2432,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2340,7 +2446,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D25" s="8"/>
     </row>
@@ -2352,7 +2458,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D26" s="8"/>
     </row>
@@ -2365,7 +2471,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2376,10 +2482,10 @@
         <v>41</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2393,7 +2499,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2417,7 +2523,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2428,7 +2534,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -2440,7 +2546,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D33" s="8"/>
     </row>
@@ -2453,7 +2559,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2478,7 +2584,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -2493,7 +2599,7 @@
         <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2504,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D38" s="8"/>
     </row>
@@ -2516,7 +2622,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -2540,13 +2646,13 @@
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>42</v>
@@ -2564,7 +2670,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="D43" s="8"/>
     </row>
@@ -2588,7 +2694,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="D45" s="8"/>
     </row>
@@ -2600,7 +2706,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="D46" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250604 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -434,10 +434,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕源,NPTV源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官方源,NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -708,6 +704,10 @@
       </rPr>
       <t>上海电信酒店源</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1176,7 +1176,7 @@
         <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>77</v>
@@ -1185,19 +1185,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
@@ -1206,52 +1206,52 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
@@ -1273,177 +1273,177 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="8"/>
@@ -1451,13 +1451,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
@@ -1473,7 +1473,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1488,7 +1488,7 @@
         <v>76</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1503,84 +1503,84 @@
         <v>76</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="1"/>
@@ -1604,7 +1604,7 @@
         <v>76</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1625,10 +1625,10 @@
         <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>76</v>
@@ -1640,10 +1640,10 @@
         <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>76</v>
@@ -1655,10 +1655,10 @@
         <v>93</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>76</v>
@@ -1670,10 +1670,10 @@
         <v>94</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>76</v>
@@ -1710,7 +1710,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2158,7 +2158,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="11" t="s">
@@ -2173,7 +2173,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2185,7 +2185,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2234,7 +2234,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2249,7 +2249,7 @@
         <v>120</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2260,7 +2260,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2272,7 +2272,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2284,10 +2284,10 @@
         <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2298,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2322,7 +2322,7 @@
         <v>40</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>110</v>
@@ -2336,7 +2336,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="8"/>
     </row>
@@ -2348,7 +2348,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2360,7 +2360,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2372,7 +2372,7 @@
         <v>40</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2384,7 +2384,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2408,7 +2408,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2420,7 +2420,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2432,10 +2432,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2446,7 +2446,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D25" s="8"/>
     </row>
@@ -2458,7 +2458,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" s="8"/>
     </row>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2499,7 +2499,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2523,7 +2523,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2534,7 +2534,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -2546,7 +2546,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="8"/>
     </row>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2584,7 +2584,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -2599,7 +2599,7 @@
         <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2610,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="8"/>
     </row>
@@ -2622,7 +2622,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -2646,7 +2646,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D41" s="8"/>
     </row>
@@ -2670,7 +2670,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="8"/>
     </row>
@@ -2694,7 +2694,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D45" s="8"/>
     </row>
@@ -2706,7 +2706,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D46" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250607 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="177">
   <si>
     <t>东方卫视</t>
   </si>
@@ -708,6 +708,14 @@
   </si>
   <si>
     <t>NPTV源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源,安徽联通酒店源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2520,7 +2528,7 @@
         <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>125</v>
@@ -2534,7 +2542,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250611 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="179">
   <si>
     <t>东方卫视</t>
   </si>
@@ -2667,7 +2667,9 @@
       <c r="B41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250611 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1173,8 +1173,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -1668,15 +1668,13 @@
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5">

</xml_diff>

<commit_message>
Update on 20250616 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="176">
   <si>
     <t>东方卫视</t>
   </si>
@@ -550,10 +550,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上海电信酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CCTV-4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -586,108 +582,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>官方源,NPTV源,安徽联通酒店源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>NPTV源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>NPTV源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>官方源,NPTV源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>官方源,NPTV源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>NPTV源,安徽联通酒店源,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上海电信酒店源</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -726,13 +620,25 @@
   <si>
     <t>咪咕源,NPTV源</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方源,NPTV源,安徽联通酒店源</t>
+  </si>
+  <si>
+    <t>NPTV源</t>
+  </si>
+  <si>
+    <t>官方源,NPTV源</t>
+  </si>
+  <si>
+    <t>NPTV源,安徽联通酒店源</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,14 +679,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -865,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1210,9 +1108,7 @@
       <c r="C2" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
@@ -1239,28 +1135,24 @@
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1271,7 +1163,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
@@ -1287,9 +1179,7 @@
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
@@ -1311,9 +1201,7 @@
       <c r="B10" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -1327,9 +1215,7 @@
       <c r="C11" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:8">
@@ -1439,7 +1325,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>75</v>
@@ -1450,7 +1336,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>144</v>
@@ -1461,7 +1347,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>144</v>
@@ -1857,12 +1743,10 @@
       <c r="B3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D3" s="1"/>
       <c r="F3" s="7"/>
       <c r="G3" s="1" t="s">
         <v>79</v>
@@ -1875,12 +1759,10 @@
       <c r="B4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D4" s="1"/>
       <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
         <v>84</v>
@@ -1903,12 +1785,10 @@
       <c r="B6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
@@ -1931,12 +1811,10 @@
       <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
@@ -1945,12 +1823,10 @@
       <c r="B9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
@@ -1986,12 +1862,10 @@
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:7">
@@ -2035,6 +1909,7 @@
       <c r="B17" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
@@ -2075,12 +1950,10 @@
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4">
@@ -2142,7 +2015,7 @@
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2187,7 +2060,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2224,7 +2097,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2235,7 +2108,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="9"/>
@@ -2251,7 +2124,7 @@
         <v>119</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2262,7 +2135,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2274,7 +2147,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2286,10 +2159,10 @@
         <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2303,7 +2176,7 @@
         <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2326,7 +2199,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>110</v>
@@ -2343,7 +2216,7 @@
         <v>120</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2354,7 +2227,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2366,7 +2239,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2390,10 +2263,10 @@
         <v>40</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2428,7 +2301,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2454,7 +2327,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="8"/>
     </row>
@@ -2528,7 +2401,7 @@
         <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>123</v>
@@ -2542,7 +2415,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -2578,7 +2451,7 @@
         <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>70</v>
@@ -2654,7 +2527,7 @@
         <v>41</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D40" s="8"/>
     </row>
@@ -2680,7 +2553,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D42" s="8"/>
     </row>
@@ -2704,7 +2577,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D44" s="8"/>
     </row>
@@ -2716,7 +2589,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D45" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250626 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="160">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1865,7 +1865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2156,13 +2158,15 @@
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="1"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -2170,10 +2174,12 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -3356,7 +3362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Update on 20250709 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="158">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1844,10 +1844,12 @@
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="H3" s="7"/>
@@ -2002,12 +2004,14 @@
         <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="1"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250711 part 7
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$F$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$G$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$C$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="154">
   <si>
     <t>东方卫视</t>
   </si>
@@ -282,10 +282,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>暂缺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>该频道仅在网络直播</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -495,17 +491,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>海南移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>黑龙江移动</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直播源来源5</t>
-  </si>
-  <si>
     <t>睛彩竞技</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -514,9 +503,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>睛彩青少</t>
-  </si>
-  <si>
     <t>睛彩广场舞</t>
   </si>
   <si>
@@ -535,10 +521,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>海南移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>黑龙江移动</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -564,6 +546,10 @@
   </si>
   <si>
     <t>直播源来源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥羊百视通</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -708,7 +694,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1010,7 +995,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1018,15 +1003,14 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -1034,488 +1018,411 @@
       <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E3" s="6"/>
+      <c r="F3" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="B23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D39"/>
+  <autoFilter ref="A1:C39"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1542,22 +1449,20 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>73</v>
@@ -1569,7 +1474,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>40</v>
@@ -1596,7 +1501,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>41</v>
@@ -1616,12 +1521,12 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>40</v>
@@ -1642,7 +1547,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>41</v>
@@ -1663,7 +1568,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>41</v>
@@ -1684,7 +1589,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>41</v>
@@ -1705,7 +1610,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>41</v>
@@ -1726,7 +1631,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>41</v>
@@ -1747,7 +1652,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>41</v>
@@ -1776,7 +1681,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1784,14 +1689,14 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -1803,41 +1708,35 @@
         <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1851,13 +1750,12 @@
         <v>77</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
@@ -1869,13 +1767,12 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4" s="11"/>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
@@ -1885,13 +1782,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5" s="6"/>
+      <c r="H5" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1903,9 +1799,8 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1919,9 +1814,8 @@
         <v>77</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1933,25 +1827,23 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>138</v>
+      <c r="C9" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
@@ -1961,9 +1853,8 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1973,9 +1864,8 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -1985,9 +1875,8 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1997,84 +1886,86 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>99</v>
+      <c r="B14" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>72</v>
@@ -2083,86 +1974,87 @@
         <v>77</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="1"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F25"/>
+  <autoFilter ref="A1:E25"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2170,7 +2062,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2181,42 +2073,38 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>41</v>
@@ -2224,16 +2112,15 @@
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2250,11 +2137,8 @@
       <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2271,11 +2155,8 @@
       <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2287,13 +2168,10 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F5" s="8"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2308,12 +2186,9 @@
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2325,13 +2200,10 @@
       <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F7" s="13"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2350,11 +2222,8 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2371,11 +2240,8 @@
       <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2394,11 +2260,8 @@
       <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2413,11 +2276,8 @@
       <c r="F11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2432,11 +2292,8 @@
       <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2455,11 +2312,8 @@
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -2474,9 +2328,8 @@
         <v>39</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2493,11 +2346,8 @@
       <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2516,11 +2366,8 @@
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2539,11 +2386,8 @@
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2562,11 +2406,8 @@
       <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2581,11 +2422,8 @@
       <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2604,11 +2442,8 @@
       <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2627,11 +2462,8 @@
       <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2650,13 +2482,10 @@
       <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>41</v>
@@ -2669,11 +2498,8 @@
       <c r="F23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2690,11 +2516,8 @@
       <c r="F24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2707,9 +2530,8 @@
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -2726,11 +2548,8 @@
       <c r="F26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2747,13 +2566,10 @@
       <c r="F27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>41</v>
@@ -2763,12 +2579,9 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2782,14 +2595,11 @@
       <c r="E29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F29" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2801,12 +2611,9 @@
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2816,12 +2623,9 @@
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -2836,11 +2640,8 @@
       <c r="F32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -2857,11 +2658,8 @@
       <c r="F33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -2878,11 +2676,8 @@
       <c r="F34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2899,11 +2694,8 @@
       <c r="F35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -2918,11 +2710,8 @@
       <c r="F36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -2939,11 +2728,8 @@
       <c r="F37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -2958,11 +2744,8 @@
       <c r="F38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
@@ -2974,12 +2757,9 @@
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -2996,26 +2776,22 @@
       <c r="F40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -3032,11 +2808,8 @@
       <c r="F42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
@@ -3051,11 +2824,8 @@
       <c r="F43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -3069,14 +2839,11 @@
         <v>39</v>
       </c>
       <c r="E44" s="8"/>
-      <c r="F44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F44" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -3093,12 +2860,9 @@
       <c r="F45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G46"/>
+  <autoFilter ref="A1:F46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3107,82 +2871,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>143</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C5"/>
+  <autoFilter ref="A1:B4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3205,7 +2947,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -3223,7 +2965,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>72</v>
@@ -3232,7 +2974,7 @@
         <v>73</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="1" t="s">
@@ -3241,7 +2983,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>72</v>
@@ -3250,12 +2992,12 @@
         <v>73</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
@@ -3264,7 +3006,7 @@
         <v>73</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20250711 part 10
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="154">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1746,10 +1746,12 @@
       <c r="C3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="8"/>
       <c r="G3" s="7"/>
       <c r="H3" s="1" t="s">
         <v>76</v>
@@ -1810,10 +1812,12 @@
       <c r="C7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
@@ -1880,10 +1884,12 @@
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="8"/>
     </row>
@@ -1979,13 +1985,15 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="1"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250712 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="155">
   <si>
     <t>东方卫视</t>
   </si>
@@ -546,6 +546,10 @@
   </si>
   <si>
     <t>直播源来源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥羊百视通</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2041,7 +2045,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2053,11 +2057,12 @@
     <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="14" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -2076,12 +2081,15 @@
       <c r="F1" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -2094,12 +2102,15 @@
       <c r="F2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2116,8 +2127,11 @@
       <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2134,8 +2148,11 @@
       <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2148,9 +2165,12 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2165,9 +2185,12 @@
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2180,9 +2203,10 @@
         <v>40</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7" s="13"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2201,8 +2225,11 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2219,8 +2246,11 @@
       <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2239,8 +2269,11 @@
       <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2255,8 +2288,11 @@
       <c r="F11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2271,8 +2307,11 @@
       <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2291,8 +2330,11 @@
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -2307,8 +2349,9 @@
         <v>39</v>
       </c>
       <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2325,8 +2368,11 @@
       <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2345,8 +2391,11 @@
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2365,8 +2414,11 @@
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2385,8 +2437,11 @@
       <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2401,8 +2456,11 @@
       <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2421,8 +2479,11 @@
       <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2441,8 +2502,11 @@
       <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2461,8 +2525,11 @@
       <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>150</v>
       </c>
@@ -2477,8 +2544,9 @@
       <c r="F23" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2495,8 +2563,11 @@
       <c r="F24" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2509,8 +2580,9 @@
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -2527,8 +2599,11 @@
       <c r="F26" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2545,8 +2620,11 @@
       <c r="F27" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>151</v>
       </c>
@@ -2559,8 +2637,9 @@
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2577,8 +2656,11 @@
       <c r="F29" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2591,8 +2673,11 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2603,8 +2688,11 @@
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -2619,8 +2707,9 @@
       <c r="F32" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -2637,8 +2726,11 @@
       <c r="F33" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -2655,8 +2747,11 @@
       <c r="F34" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2673,8 +2768,11 @@
       <c r="F35" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -2689,8 +2787,11 @@
       <c r="F36" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -2707,8 +2808,11 @@
       <c r="F37" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -2723,8 +2827,11 @@
       <c r="F38" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
@@ -2737,8 +2844,9 @@
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -2755,8 +2863,11 @@
       <c r="F40" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G40" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
@@ -2769,8 +2880,9 @@
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -2787,8 +2899,11 @@
       <c r="F42" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G42" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
@@ -2803,8 +2918,9 @@
       <c r="F43" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -2821,8 +2937,11 @@
       <c r="F44" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G44" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -2839,9 +2958,11 @@
       <c r="F45" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="G45" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250712 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="155">
   <si>
     <t>东方卫视</t>
   </si>
@@ -2349,7 +2349,9 @@
         <v>39</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250712 part 7
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -15,10 +15,10 @@
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$G$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$C$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="156">
   <si>
     <t>东方卫视</t>
   </si>
@@ -546,6 +546,10 @@
   </si>
   <si>
     <t>直播源来源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥羊百视通</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1435,7 +1439,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1445,12 +1449,14 @@
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -1466,15 +1472,18 @@
       <c r="E1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>79</v>
       </c>
@@ -1490,15 +1499,16 @@
       <c r="E2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
@@ -1515,12 +1525,15 @@
       <c r="F3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>81</v>
       </c>
@@ -1534,11 +1547,14 @@
       <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -1554,9 +1570,10 @@
       <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F5" s="8"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -1572,9 +1589,10 @@
       <c r="E6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F6" s="8"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -1590,9 +1608,10 @@
       <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F7" s="8"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
@@ -1608,9 +1627,10 @@
       <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F8" s="8"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -1626,9 +1646,10 @@
       <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F9" s="8"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
@@ -1644,10 +1665,11 @@
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F10"/>
+  <autoFilter ref="A1:G10"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2846,7 +2868,9 @@
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="G39" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
@@ -2965,6 +2989,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G45"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250720 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$G$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$C$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="158">
   <si>
     <t>东方卫视</t>
   </si>
@@ -427,10 +427,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>安徽联通酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CGTN英语</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -455,10 +451,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>湖北电信酒店源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -562,6 +554,18 @@
   </si>
   <si>
     <t>睛彩青少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥羊yhyx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源来源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源来源4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -662,7 +666,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -685,11 +689,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -706,6 +723,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1007,22 +1028,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="16" customWidth="1"/>
     <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -1030,12 +1053,18 @@
       <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="E1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -1043,14 +1072,16 @@
         <v>72</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>105</v>
       </c>
@@ -1058,14 +1089,16 @@
         <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>106</v>
       </c>
@@ -1073,39 +1106,47 @@
         <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D6" s="8"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D7" s="8"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -1113,10 +1154,12 @@
         <v>72</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>119</v>
       </c>
@@ -1124,10 +1167,12 @@
         <v>72</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -1135,10 +1180,12 @@
         <v>120</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -1146,10 +1193,12 @@
         <v>72</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
@@ -1157,10 +1206,12 @@
         <v>72</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>111</v>
       </c>
@@ -1168,10 +1219,12 @@
         <v>72</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>112</v>
       </c>
@@ -1179,10 +1232,12 @@
         <v>72</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>113</v>
       </c>
@@ -1190,10 +1245,12 @@
         <v>72</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>114</v>
       </c>
@@ -1201,10 +1258,12 @@
         <v>72</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
@@ -1212,10 +1271,12 @@
         <v>72</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>116</v>
       </c>
@@ -1223,10 +1284,12 @@
         <v>72</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>117</v>
       </c>
@@ -1234,10 +1297,12 @@
         <v>72</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
@@ -1245,39 +1310,47 @@
         <v>120</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D22" s="8"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D23" s="8"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -1285,119 +1358,167 @@
         <v>73</v>
       </c>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D24" s="8"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C25" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C26" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C27" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C28" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C29" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C31" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C32" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C33" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C34" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C35" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -1405,8 +1526,10 @@
         <v>72</v>
       </c>
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D36" s="8"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>96</v>
       </c>
@@ -1414,8 +1537,10 @@
         <v>72</v>
       </c>
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D37" s="8"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>97</v>
       </c>
@@ -1423,8 +1548,10 @@
         <v>72</v>
       </c>
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D38" s="8"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
@@ -1432,9 +1559,11 @@
         <v>98</v>
       </c>
       <c r="C39" s="1"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C39"/>
+  <autoFilter ref="A1:E39"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1462,22 +1591,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>73</v>
@@ -1534,7 +1663,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -1560,7 +1689,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>41</v>
@@ -1579,7 +1708,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>41</v>
@@ -1598,7 +1727,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>41</v>
@@ -1617,7 +1746,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>41</v>
@@ -1636,7 +1765,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>41</v>
@@ -1655,7 +1784,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>41</v>
@@ -1697,7 +1826,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -1709,7 +1838,7 @@
         <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>74</v>
@@ -1727,7 +1856,7 @@
         <v>120</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>77</v>
@@ -1748,7 +1877,7 @@
         <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>77</v>
@@ -1787,7 +1916,7 @@
       <c r="E5" s="8"/>
       <c r="G5" s="6"/>
       <c r="H5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -1814,7 +1943,7 @@
         <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>77</v>
@@ -1841,7 +1970,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>77</v>
@@ -1886,7 +2015,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>77</v>
@@ -1899,7 +2028,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>98</v>
@@ -1916,7 +2045,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>77</v>
@@ -1929,7 +2058,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>71</v>
@@ -1944,7 +2073,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>77</v>
@@ -1957,7 +2086,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>72</v>
@@ -1987,7 +2116,7 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>98</v>
@@ -2002,7 +2131,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>77</v>
@@ -2015,7 +2144,7 @@
         <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>77</v>
@@ -2028,7 +2157,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>77</v>
@@ -2041,7 +2170,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>72</v>
@@ -2056,7 +2185,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
@@ -2090,25 +2219,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>145</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>74</v>
@@ -2117,7 +2246,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>41</v>
@@ -2133,7 +2262,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -2561,7 +2690,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>41</v>
@@ -2656,7 +2785,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>41</v>
@@ -2911,7 +3040,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -3022,10 +3151,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>74</v>
@@ -3034,38 +3163,38 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3092,7 +3221,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Update on 20250721 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$I$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="158">
   <si>
     <t>东方卫视</t>
   </si>
@@ -526,52 +526,44 @@
     <t>农林卫视</t>
   </si>
   <si>
+    <t>睛彩青少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源来源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CETV-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百视通</t>
+  </si>
+  <si>
+    <t>NPTV</t>
+  </si>
+  <si>
+    <t>GPTV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPTV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银河有线</t>
+  </si>
+  <si>
+    <t>直播源来源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>直播源来源2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>睛彩青少</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源来源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源来源4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CETV-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yhyx</t>
-  </si>
-  <si>
-    <t>百视通</t>
-  </si>
-  <si>
-    <t>NPTV</t>
-  </si>
-  <si>
-    <t>GPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yhyx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yhyx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东方卫视</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -626,7 +618,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,12 +634,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,26 +690,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1027,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1035,14 +1020,13 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -1053,77 +1037,70 @@
         <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="6"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="6"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -1131,10 +1108,9 @@
         <v>72</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>129</v>
       </c>
@@ -1142,205 +1118,189 @@
         <v>72</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C22" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>132</v>
       </c>
@@ -1348,10 +1308,9 @@
         <v>119</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
@@ -1359,169 +1318,153 @@
         <v>73</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>157</v>
+      <c r="C25" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>152</v>
+      <c r="C27" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>152</v>
+      <c r="C28" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C29" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>152</v>
+      <c r="C30" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C31" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>152</v>
+      <c r="C33" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C34" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C35" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>94</v>
       </c>
@@ -1529,10 +1472,9 @@
         <v>72</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
@@ -1540,10 +1482,9 @@
         <v>72</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
@@ -1551,10 +1492,9 @@
         <v>72</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>93</v>
       </c>
@@ -1562,11 +1502,10 @@
         <v>97</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="1"/>
+      <c r="D39" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39"/>
+  <autoFilter ref="A1:D39"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1577,9 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1603,22 +1540,22 @@
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>155</v>
+      <c r="H1" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>74</v>
@@ -1641,12 +1578,12 @@
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="J2" s="10"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1655,7 +1592,7 @@
       <c r="A3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="1"/>
@@ -1672,28 +1609,28 @@
         <v>40</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
@@ -1721,7 +1658,7 @@
       <c r="A6" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1733,7 +1670,7 @@
       <c r="E6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -1741,7 +1678,7 @@
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1753,7 +1690,7 @@
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
@@ -1761,7 +1698,7 @@
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1773,7 +1710,7 @@
       <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -1781,7 +1718,7 @@
       <c r="A9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1793,7 +1730,7 @@
       <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
@@ -1801,7 +1738,7 @@
       <c r="A10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1813,7 +1750,7 @@
       <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
@@ -1821,7 +1758,7 @@
       <c r="A11" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1833,7 +1770,7 @@
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -1887,7 +1824,7 @@
       <c r="C2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="2"/>
@@ -1906,9 +1843,9 @@
         <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
         <v>76</v>
       </c>
@@ -1922,13 +1859,13 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1936,7 +1873,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1962,7 +1899,7 @@
         <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -1983,12 +1920,12 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2022,7 +1959,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2032,10 +1969,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>150</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>73</v>
@@ -2046,7 +1983,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2056,7 +1993,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>71</v>
@@ -2068,9 +2005,11 @@
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -2078,7 +2017,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>72</v>
@@ -2102,10 +2041,10 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>97</v>
@@ -2116,9 +2055,11 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -2126,9 +2067,11 @@
         <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -2136,9 +2079,11 @@
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -2146,21 +2091,23 @@
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="C25" s="6"/>
       <c r="D25" s="1"/>
     </row>
   </sheetData>
@@ -2184,10 +2131,10 @@
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="13" customWidth="1"/>
     <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
@@ -2203,24 +2150,24 @@
         <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" s="15" t="s">
+      <c r="I1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>74</v>
       </c>
       <c r="L1" s="1"/>
@@ -2229,12 +2176,12 @@
       <c r="A2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
@@ -2244,8 +2191,8 @@
       <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="6"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="1" t="s">
         <v>133</v>
       </c>
@@ -2314,8 +2261,8 @@
       <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
@@ -2328,7 +2275,7 @@
       <c r="I5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
@@ -2337,7 +2284,7 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
@@ -2351,31 +2298,31 @@
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="K6" s="11"/>
+      <c r="I6" s="6"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="8"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -2401,8 +2348,8 @@
       <c r="I8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="8"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
@@ -2446,7 +2393,7 @@
       <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
@@ -2496,11 +2443,11 @@
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2521,11 +2468,11 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
@@ -2572,7 +2519,7 @@
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2582,12 +2529,12 @@
       <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
@@ -2602,7 +2549,7 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2710,11 +2657,11 @@
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
@@ -2782,7 +2729,7 @@
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
@@ -2817,22 +2764,22 @@
       <c r="A24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="7"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
@@ -2847,7 +2794,7 @@
       <c r="D25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
@@ -2865,19 +2812,19 @@
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="20"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
@@ -2892,7 +2839,7 @@
       <c r="D27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
@@ -2919,7 +2866,7 @@
       <c r="D28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2937,21 +2884,21 @@
       <c r="A29" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
       <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="20"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
@@ -2990,52 +2937,52 @@
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
       <c r="G31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
       <c r="G32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="7"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="7"/>
+      <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
@@ -3050,7 +2997,7 @@
       <c r="D34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="1" t="s">
         <v>39</v>
       </c>
@@ -3077,7 +3024,7 @@
       <c r="D35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="7"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="2" t="s">
         <v>40</v>
       </c>
@@ -3156,7 +3103,7 @@
       <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="1" t="s">
         <v>39</v>
       </c>
@@ -3164,7 +3111,7 @@
         <v>39</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="7"/>
+      <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
@@ -3173,11 +3120,11 @@
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="6"/>
       <c r="F39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3195,20 +3142,20 @@
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="7"/>
+      <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
@@ -3223,7 +3170,7 @@
       <c r="D41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
@@ -3241,19 +3188,19 @@
       <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="20"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="19"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
@@ -3268,7 +3215,7 @@
       <c r="D43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
@@ -3286,22 +3233,22 @@
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="7"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="7"/>
+      <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
@@ -3316,7 +3263,7 @@
       <c r="D45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="2" t="s">
         <v>40</v>
       </c>
@@ -3343,7 +3290,7 @@
       <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="1" t="s">
         <v>39</v>
       </c>
@@ -3384,7 +3331,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>74</v>
@@ -3392,30 +3339,30 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3423,7 +3370,7 @@
       <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3457,7 +3404,7 @@
         <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>66</v>
@@ -3468,17 +3415,17 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
@@ -3486,31 +3433,31 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20250722 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="155">
   <si>
     <t>东方卫视</t>
   </si>
@@ -228,16 +228,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直播源来源1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源来源2</t>
-  </si>
-  <si>
-    <t>直播源来源3</t>
-  </si>
-  <si>
     <t>官方源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -254,10 +244,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>酒店源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>咪咕源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,10 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>暂时失效源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>该频道仅在网络直播</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -530,10 +512,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直播源来源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CETV-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -559,12 +537,20 @@
     <t>银河有线</t>
   </si>
   <si>
-    <t>直播源来源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源来源2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>NPTV,咪咕源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源1</t>
+  </si>
+  <si>
+    <t>直播源2</t>
+  </si>
+  <si>
+    <t>直播源3</t>
+  </si>
+  <si>
+    <t>直播源</t>
   </si>
 </sst>
 </file>
@@ -618,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,12 +614,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,25 +670,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1019,490 +997,539 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="12" customWidth="1"/>
     <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>74</v>
+        <v>153</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="F2" s="15"/>
+        <v>98</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="14"/>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="F3" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="15"/>
       <c r="G3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>102</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="6"/>
+        <v>104</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>105</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>107</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="6"/>
+        <v>109</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="6"/>
+        <v>110</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>112</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>155</v>
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>152</v>
+        <v>69</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>155</v>
+        <v>69</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="6"/>
+      <c r="D39" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D39"/>
@@ -1534,37 +1561,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
@@ -1578,19 +1605,19 @@
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="J2" s="9"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -1611,30 +1638,29 @@
       <c r="H3" s="1"/>
       <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="18"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1656,7 +1682,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
@@ -1670,13 +1696,13 @@
       <c r="E6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
@@ -1690,13 +1716,13 @@
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
@@ -1710,13 +1736,13 @@
       <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -1730,13 +1756,13 @@
       <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>
@@ -1750,13 +1776,13 @@
       <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
@@ -1770,7 +1796,7 @@
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -1791,26 +1817,28 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1819,17 +1847,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1837,17 +1865,17 @@
         <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1855,37 +1883,39 @@
         <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="1" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
-        <v>69</v>
+      <c r="A5" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -1893,13 +1923,13 @@
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -1907,31 +1937,35 @@
         <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -1939,7 +1973,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1949,7 +1983,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1959,7 +1993,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1969,13 +2003,13 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -1983,7 +2017,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1993,11 +2027,9 @@
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -2005,10 +2037,10 @@
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2017,10 +2049,10 @@
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2029,10 +2061,10 @@
         <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2041,24 +2073,22 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2067,10 +2097,10 @@
         <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2079,10 +2109,10 @@
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2091,13 +2121,13 @@
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -2105,9 +2135,9 @@
         <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="1"/>
     </row>
   </sheetData>
@@ -2131,57 +2161,57 @@
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="12" customWidth="1"/>
     <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>74</v>
+        <v>136</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
@@ -2191,10 +2221,10 @@
       <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="K2" s="16"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -2261,8 +2291,8 @@
       <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
@@ -2275,7 +2305,7 @@
       <c r="I5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
@@ -2284,7 +2314,7 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
@@ -2298,8 +2328,8 @@
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="5"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
@@ -2308,21 +2338,21 @@
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="7"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -2348,8 +2378,8 @@
       <c r="I8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
@@ -2393,7 +2423,7 @@
       <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
@@ -2443,11 +2473,11 @@
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
@@ -2468,11 +2498,11 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
@@ -2529,12 +2559,12 @@
       <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
@@ -2549,7 +2579,7 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2657,11 +2687,11 @@
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
@@ -2729,7 +2759,7 @@
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
@@ -2762,7 +2792,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>41</v>
@@ -2770,16 +2800,16 @@
       <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
@@ -2794,7 +2824,7 @@
       <c r="D25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
@@ -2818,13 +2848,13 @@
       <c r="C26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="19"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
@@ -2839,7 +2869,7 @@
       <c r="D27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
@@ -2866,7 +2896,7 @@
       <c r="D28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2882,7 +2912,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>41</v>
@@ -2890,15 +2920,15 @@
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="19"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
@@ -2937,16 +2967,16 @@
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="6"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
@@ -2955,15 +2985,15 @@
       <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="6"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
@@ -2975,14 +3005,14 @@
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="6"/>
+      <c r="G33" s="5"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="6"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
@@ -2997,7 +3027,7 @@
       <c r="D34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="1" t="s">
         <v>39</v>
       </c>
@@ -3024,7 +3054,7 @@
       <c r="D35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="2" t="s">
         <v>40</v>
       </c>
@@ -3103,7 +3133,7 @@
       <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="1" t="s">
         <v>39</v>
       </c>
@@ -3111,7 +3141,7 @@
         <v>39</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="6"/>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
@@ -3120,11 +3150,11 @@
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3148,14 +3178,14 @@
       <c r="C40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
       <c r="G40" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="6"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
@@ -3170,7 +3200,7 @@
       <c r="D41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
@@ -3186,21 +3216,21 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+        <v>138</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
@@ -3215,7 +3245,7 @@
       <c r="D43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
@@ -3239,16 +3269,16 @@
       <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="6"/>
+      <c r="G44" s="5"/>
       <c r="H44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="6"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
@@ -3263,7 +3293,7 @@
       <c r="D45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="2" t="s">
         <v>40</v>
       </c>
@@ -3290,7 +3320,7 @@
       <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="6"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="1" t="s">
         <v>39</v>
       </c>
@@ -3320,58 +3350,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>135</v>
+      <c r="A2" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>136</v>
+      <c r="A3" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3391,73 +3420,74 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>100</v>
+      <c r="A2" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>155</v>
+        <v>68</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>98</v>
+      <c r="A3" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>155</v>
+        <v>68</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>99</v>
+      <c r="A4" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>155</v>
+        <v>68</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20250724 part 21
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -18,16 +18,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$I$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="155">
   <si>
     <t>东方卫视</t>
   </si>
@@ -534,9 +534,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>银河有线</t>
-  </si>
-  <si>
     <t>NPTV,咪咕源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -551,6 +548,10 @@
   </si>
   <si>
     <t>直播源</t>
+  </si>
+  <si>
+    <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -998,8 +999,8 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.125" style="12" customWidth="1"/>
     <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
@@ -1010,13 +1011,13 @@
         <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>70</v>
@@ -1317,9 +1318,7 @@
       <c r="C22" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
@@ -1348,12 +1347,10 @@
       <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
@@ -1365,9 +1362,7 @@
       <c r="C26" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
@@ -1379,9 +1374,7 @@
       <c r="C27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
@@ -1393,9 +1386,7 @@
       <c r="C28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
@@ -1404,9 +1395,7 @@
       <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -1419,9 +1408,7 @@
       <c r="C30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
@@ -1430,9 +1417,7 @@
       <c r="B31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -1442,9 +1427,7 @@
       <c r="B32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -1454,12 +1437,10 @@
       <c r="B33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
@@ -1468,9 +1449,7 @@
       <c r="B34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -1480,9 +1459,7 @@
       <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
@@ -1829,13 +1806,13 @@
         <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
@@ -1850,7 +1827,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>129</v>
@@ -2005,10 +1982,7 @@
       <c r="B14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2039,9 +2013,7 @@
       <c r="B17" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -2075,9 +2047,7 @@
       <c r="B20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -2087,9 +2057,7 @@
       <c r="B21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -2099,9 +2067,7 @@
       <c r="B22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -2111,9 +2077,7 @@
       <c r="B23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -2123,10 +2087,7 @@
       <c r="B24" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2149,7 +2110,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2163,13 +2124,12 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>134</v>
       </c>
@@ -2194,15 +2154,12 @@
       <c r="H1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2221,13 +2178,12 @@
       <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2250,11 +2206,8 @@
       <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2277,11 +2230,8 @@
       <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2302,12 +2252,9 @@
       <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2328,10 +2275,9 @@
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2346,11 +2292,10 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I7" s="17"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>148</v>
       </c>
@@ -2375,13 +2320,10 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I8" s="17"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2406,11 +2348,8 @@
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2433,11 +2372,8 @@
       <c r="H10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2462,11 +2398,8 @@
       <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2487,11 +2420,8 @@
       <c r="H12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2512,11 +2442,8 @@
       <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2541,11 +2468,8 @@
       <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2564,9 +2488,8 @@
         <v>39</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2589,11 +2512,8 @@
       <c r="H16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2618,11 +2538,8 @@
       <c r="H17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2647,11 +2564,8 @@
       <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2676,11 +2590,8 @@
       <c r="H19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2701,11 +2612,8 @@
       <c r="H20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -2730,11 +2638,8 @@
       <c r="H21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2759,9 +2664,8 @@
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2786,11 +2690,8 @@
       <c r="H23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>140</v>
       </c>
@@ -2809,9 +2710,8 @@
       <c r="H24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -2834,11 +2734,8 @@
       <c r="H25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -2853,10 +2750,9 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2879,11 +2775,8 @@
       <c r="H27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2906,11 +2799,8 @@
       <c r="H28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>141</v>
       </c>
@@ -2927,10 +2817,9 @@
       <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -2953,11 +2842,8 @@
         <v>40</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -2976,9 +2862,8 @@
       <c r="H31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2993,9 +2878,8 @@
         <v>40</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3012,9 +2896,8 @@
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3037,11 +2920,8 @@
       <c r="H34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -3062,11 +2942,8 @@
         <v>40</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -3091,11 +2968,8 @@
       <c r="H36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -3116,11 +2990,8 @@
       <c r="H37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -3141,9 +3012,8 @@
         <v>39</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -3164,11 +3034,8 @@
       <c r="H39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -3185,9 +3052,8 @@
         <v>40</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -3210,11 +3076,8 @@
       <c r="H41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>96</v>
       </c>
@@ -3229,10 +3092,9 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="17"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -3255,11 +3117,8 @@
       <c r="H43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -3278,9 +3137,8 @@
       <c r="H44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -3303,11 +3161,8 @@
       <c r="H45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -3330,12 +3185,9 @@
       <c r="H46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I46"/>
+  <autoFilter ref="A1:H46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3360,7 +3212,7 @@
         <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>70</v>
@@ -3413,85 +3265,73 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D4"/>
+  <autoFilter ref="A1:C4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20250726 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -20,14 +20,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -550,7 +550,15 @@
     <t>直播源</t>
   </si>
   <si>
+    <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1526,9 +1534,9 @@
   <cols>
     <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
@@ -1543,17 +1551,17 @@
       <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>69</v>
@@ -1573,16 +1581,16 @@
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="5"/>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1599,15 +1607,15 @@
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>40</v>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>40</v>
@@ -1642,13 +1650,13 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
@@ -1664,16 +1672,16 @@
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="5"/>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -1684,16 +1692,16 @@
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
@@ -1704,16 +1712,16 @@
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="5"/>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -1724,16 +1732,16 @@
       <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5"/>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
@@ -1744,16 +1752,16 @@
       <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="5"/>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
@@ -1764,16 +1772,16 @@
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5"/>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -2119,12 +2127,11 @@
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="9" width="9.125" style="12" customWidth="1"/>
     <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
@@ -2139,20 +2146,20 @@
       <c r="C1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>70</v>
@@ -2167,17 +2174,18 @@
         <v>41</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="15"/>
       <c r="K2" s="1" t="s">
         <v>128</v>
@@ -2196,16 +2204,16 @@
       <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
@@ -2220,16 +2228,16 @@
       <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
@@ -2241,17 +2249,17 @@
       <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -2265,16 +2273,16 @@
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H6" s="1"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -2286,13 +2294,12 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="17"/>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -2320,7 +2327,6 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="17"/>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -2359,19 +2365,19 @@
       <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
@@ -2410,16 +2416,16 @@
       <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
@@ -2432,16 +2438,16 @@
       <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
@@ -2456,8 +2462,8 @@
       <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>40</v>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>39</v>
@@ -2465,8 +2471,8 @@
       <c r="G14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>39</v>
+      <c r="H14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -2479,15 +2485,15 @@
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
@@ -2502,16 +2508,16 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
@@ -2526,8 +2532,8 @@
       <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>40</v>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
@@ -2535,8 +2541,8 @@
       <c r="G17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>39</v>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -2602,16 +2608,16 @@
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
@@ -2626,8 +2632,8 @@
       <c r="D21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>40</v>
+      <c r="E21" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>39</v>
@@ -2635,8 +2641,8 @@
       <c r="G21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>39</v>
+      <c r="H21" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
@@ -2701,15 +2707,16 @@
       <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
@@ -2724,16 +2731,16 @@
       <c r="D25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
@@ -2747,9 +2754,9 @@
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
@@ -2762,19 +2769,19 @@
       <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="5"/>
+      <c r="D27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
@@ -2786,19 +2793,19 @@
       <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="5"/>
+      <c r="D28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
@@ -2812,11 +2819,11 @@
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="F29" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G29" s="10"/>
-      <c r="H29" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="H29" s="10"/>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
@@ -2829,19 +2836,19 @@
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>39</v>
+      <c r="D30" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
@@ -2854,14 +2861,14 @@
         <v>39</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="E31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
@@ -2872,12 +2879,13 @@
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="1"/>
+      <c r="E32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
@@ -2889,13 +2897,14 @@
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
@@ -2910,16 +2919,16 @@
       <c r="D34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
@@ -2931,17 +2940,17 @@
       <c r="C35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="1"/>
+      <c r="D35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
@@ -2953,17 +2962,17 @@
       <c r="C36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>40</v>
+      <c r="D36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>39</v>
@@ -2980,16 +2989,16 @@
       <c r="D37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
@@ -3004,14 +3013,14 @@
       <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="E38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
@@ -3024,16 +3033,16 @@
       <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
@@ -3046,12 +3055,13 @@
         <v>39</v>
       </c>
       <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H40" s="1"/>
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
@@ -3063,19 +3073,19 @@
       <c r="C41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="5"/>
+      <c r="D41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
@@ -3089,9 +3099,9 @@
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="1"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="1"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
@@ -3104,19 +3114,19 @@
       <c r="C43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
@@ -3128,15 +3138,16 @@
       <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="D44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="5"/>
       <c r="F44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
@@ -3148,19 +3159,19 @@
       <c r="C45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="2" t="s">
-        <v>40</v>
+      <c r="D45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
@@ -3175,16 +3186,16 @@
       <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F46" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H46" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H46"/>
@@ -3265,73 +3276,85 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>69</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C4"/>
+  <autoFilter ref="A1:D4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20250726 part 7
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1620,7 +1620,9 @@
       <c r="G3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
         <v>128</v>
@@ -1663,7 +1665,9 @@
       <c r="G5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250727 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1874,10 +1874,12 @@
       <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="F4" s="4"/>
       <c r="G4" s="1" t="s">
         <v>128</v>
@@ -1902,10 +1904,12 @@
       <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
@@ -1928,10 +1932,12 @@
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
@@ -1995,6 +2001,9 @@
         <v>144</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250731 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="央视" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="160">
   <si>
     <t>东方卫视</t>
   </si>
@@ -652,7 +652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -688,22 +688,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -722,7 +711,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1031,9 +1019,9 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.125" style="12" customWidth="1"/>
     <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
@@ -1053,7 +1041,7 @@
       <c r="D1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="5" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="13" t="s">
@@ -1141,26 +1129,26 @@
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -1384,9 +1372,7 @@
       <c r="A21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>157</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
         <v>128</v>
       </c>
@@ -1401,23 +1387,23 @@
       <c r="A22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>145</v>
       </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="5"/>
     </row>
@@ -1425,10 +1411,10 @@
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="5"/>
     </row>
@@ -1436,182 +1422,182 @@
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>145</v>
       </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="1"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="5"/>
     </row>
@@ -1627,9 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1686,7 +1670,9 @@
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1760,7 +1746,9 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
@@ -1785,7 +1773,9 @@
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
@@ -2289,6 +2279,7 @@
       <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
@@ -2718,9 +2709,7 @@
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="10"/>
       <c r="F15" s="1" t="s">
         <v>39</v>
@@ -2967,7 +2956,9 @@
       <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
@@ -3108,8 +3099,8 @@
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>40</v>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>40</v>
@@ -3225,8 +3216,8 @@
       <c r="C35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>40</v>
+      <c r="D35" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Update on 20250731 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="央视" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="160">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1238,7 +1238,9 @@
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>128</v>
       </c>
@@ -1372,7 +1374,9 @@
       <c r="A21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>128</v>
       </c>
@@ -1387,13 +1391,15 @@
       <c r="A22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="1"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -1699,7 +1705,9 @@
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1746,8 +1754,8 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>40</v>
@@ -2115,7 +2123,9 @@
       <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
@@ -2123,10 +2133,12 @@
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
@@ -2134,11 +2146,11 @@
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>91</v>
@@ -2151,11 +2163,11 @@
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2164,11 +2176,11 @@
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2177,11 +2189,11 @@
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="1"/>
@@ -2190,11 +2202,11 @@
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>67</v>
@@ -2208,21 +2220,21 @@
       <c r="B19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
@@ -2231,11 +2243,11 @@
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
@@ -2244,11 +2256,11 @@
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
@@ -2257,11 +2269,11 @@
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
@@ -2270,11 +2282,11 @@
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>67</v>
@@ -2303,7 +2315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3025,8 +3037,8 @@
       <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>40</v>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>40</v>
@@ -3439,7 +3451,9 @@
       <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E44" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250802 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="14805" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="央视" sheetId="3" r:id="rId1"/>
@@ -692,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -707,7 +707,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1044,7 +1043,7 @@
       <c r="E1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="H1" s="1"/>
@@ -1065,7 +1064,7 @@
       <c r="E2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
         <v>70</v>
       </c>
@@ -1086,7 +1085,7 @@
       <c r="E3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="1" t="s">
         <v>127</v>
       </c>
@@ -1172,16 +1171,16 @@
       <c r="A9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
@@ -1745,7 +1744,7 @@
       <c r="I4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
@@ -2315,7 +2314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2387,8 +2386,8 @@
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="1" t="s">
         <v>127</v>
       </c>
@@ -2980,7 +2979,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="17"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
@@ -3025,7 +3024,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="17"/>
+      <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
@@ -3099,7 +3098,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="17"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
@@ -3169,7 +3168,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
@@ -3189,7 +3188,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
@@ -3367,7 +3366,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="17"/>
+      <c r="J40" s="16"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
@@ -3412,7 +3411,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="17"/>
+      <c r="J42" s="16"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
@@ -3463,7 +3462,7 @@
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
-      <c r="J44" s="17"/>
+      <c r="J44" s="16"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250802 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$I$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$I$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="158">
   <si>
     <t>东方卫视</t>
   </si>
@@ -196,9 +196,6 @@
     <t>欢笑剧场</t>
   </si>
   <si>
-    <t>魅力足球</t>
-  </si>
-  <si>
     <t>劲爆体育</t>
   </si>
   <si>
@@ -517,10 +514,6 @@
   </si>
   <si>
     <t>NPTV</t>
-  </si>
-  <si>
-    <t>GPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GPTV</t>
@@ -1029,384 +1022,384 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1414,10 +1407,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1425,62 +1418,62 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="1"/>
@@ -1488,23 +1481,23 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="1"/>
@@ -1512,10 +1505,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="1"/>
@@ -1523,23 +1516,23 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="1"/>
@@ -1547,10 +1540,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="1"/>
@@ -1558,49 +1551,49 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1637,40 +1630,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
@@ -1694,12 +1687,12 @@
       <c r="I2" s="1"/>
       <c r="K2" s="8"/>
       <c r="L2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -1725,12 +1718,12 @@
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -1748,7 +1741,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1775,7 +1768,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
@@ -1798,7 +1791,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
@@ -1819,7 +1812,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
@@ -1840,7 +1833,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -1861,7 +1854,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>
@@ -1882,7 +1875,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
@@ -1911,7 +1904,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1928,22 +1921,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -1952,74 +1945,74 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2028,16 +2021,16 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -2045,16 +2038,16 @@
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -2062,55 +2055,55 @@
         <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2120,10 +2113,10 @@
         <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2133,10 +2126,10 @@
         <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2146,16 +2139,16 @@
         <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -2163,10 +2156,10 @@
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2176,10 +2169,10 @@
         <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2189,10 +2182,10 @@
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="1"/>
@@ -2202,13 +2195,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -2216,13 +2209,13 @@
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>91</v>
+      <c r="B19" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -2230,10 +2223,10 @@
         <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
@@ -2243,10 +2236,10 @@
         <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
@@ -2256,10 +2249,10 @@
         <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
@@ -2269,42 +2262,29 @@
         <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>142</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="B24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E25"/>
+  <autoFilter ref="A1:E24"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2312,7 +2292,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2324,49 +2304,45 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="9" width="9.125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
@@ -2381,18 +2357,15 @@
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I2" s="16"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2414,12 +2387,9 @@
       <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2441,12 +2411,9 @@
       <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2465,14 +2432,11 @@
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2492,13 +2456,10 @@
       <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H6" s="1"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2509,16 +2470,15 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G7" s="10"/>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -2541,12 +2501,9 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2571,11 +2528,8 @@
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2594,15 +2548,12 @@
       <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2627,11 +2578,8 @@
       <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2651,12 +2599,9 @@
       <c r="G12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2676,12 +2621,9 @@
       <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2703,14 +2645,11 @@
       <c r="G14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2726,12 +2665,11 @@
         <v>39</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2753,12 +2691,9 @@
       <c r="G16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2780,14 +2715,11 @@
       <c r="G17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2812,11 +2744,8 @@
       <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2841,11 +2770,8 @@
       <c r="H19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2865,12 +2791,9 @@
       <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -2892,14 +2815,11 @@
       <c r="G21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2924,11 +2844,8 @@
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2953,13 +2870,10 @@
       <c r="H23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>41</v>
@@ -2974,14 +2888,11 @@
         <v>40</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -3003,12 +2914,9 @@
       <c r="G25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -3021,12 +2929,11 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -3045,15 +2952,12 @@
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -3072,17 +2976,14 @@
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>41</v>
@@ -3093,14 +2994,11 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -3119,15 +3017,14 @@
       <c r="F30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -3144,13 +3041,10 @@
       <c r="F31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3165,12 +3059,11 @@
       <c r="F32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="16"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3185,12 +3078,11 @@
         <v>40</v>
       </c>
       <c r="F33" s="5"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3212,12 +3104,9 @@
       <c r="G34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -3236,13 +3125,12 @@
       <c r="F35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -3267,11 +3155,8 @@
       <c r="H36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -3291,12 +3176,9 @@
       <c r="G37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -3315,13 +3197,12 @@
       <c r="F38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -3341,12 +3222,9 @@
       <c r="G39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -3363,12 +3241,11 @@
       <c r="F40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -3387,33 +3264,29 @@
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="1"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -3432,15 +3305,12 @@
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -3457,14 +3327,11 @@
         <v>40</v>
       </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G44" s="10"/>
       <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -3486,12 +3353,9 @@
       <c r="G45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -3513,13 +3377,10 @@
       <c r="G46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I46" s="5"/>
+      <c r="H46" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I46"/>
+  <autoFilter ref="A1:H46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3541,50 +3402,50 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3612,66 +3473,66 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20250802 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="158">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1779,7 +1779,9 @@
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250805 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$I$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$B$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="159">
   <si>
     <t>东方卫视</t>
   </si>
@@ -537,9 +537,6 @@
     <t>直播源3</t>
   </si>
   <si>
-    <t>直播源</t>
-  </si>
-  <si>
     <t>直播源1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -565,6 +562,14 @@
   </si>
   <si>
     <t>东方购物一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1034,7 +1039,7 @@
         <v>149</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>68</v>
@@ -1046,7 +1051,7 @@
         <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>127</v>
@@ -1067,7 +1072,7 @@
         <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>127</v>
@@ -1088,7 +1093,7 @@
         <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>127</v>
@@ -1105,7 +1110,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>127</v>
@@ -1148,7 +1153,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>127</v>
@@ -1180,7 +1185,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>127</v>
@@ -1197,7 +1202,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>127</v>
@@ -1214,7 +1219,7 @@
         <v>102</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>127</v>
@@ -1231,7 +1236,7 @@
         <v>103</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>127</v>
@@ -1248,7 +1253,7 @@
         <v>104</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>127</v>
@@ -1265,7 +1270,7 @@
         <v>105</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>127</v>
@@ -1282,7 +1287,7 @@
         <v>106</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>127</v>
@@ -1299,7 +1304,7 @@
         <v>107</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>127</v>
@@ -1316,7 +1321,7 @@
         <v>108</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>127</v>
@@ -1333,7 +1338,7 @@
         <v>109</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>127</v>
@@ -1350,7 +1355,7 @@
         <v>110</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>127</v>
@@ -1367,7 +1372,7 @@
         <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>127</v>
@@ -1384,7 +1389,7 @@
         <v>124</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>142</v>
@@ -1636,7 +1641,7 @@
         <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>127</v>
@@ -1935,7 +1940,7 @@
         <v>149</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>68</v>
@@ -1950,7 +1955,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>146</v>
@@ -1971,7 +1976,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>66</v>
@@ -1992,7 +1997,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>142</v>
@@ -2026,7 +2031,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>142</v>
@@ -2043,7 +2048,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>66</v>
@@ -2060,7 +2065,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>142</v>
@@ -2077,7 +2082,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>142</v>
@@ -2099,13 +2104,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2118,7 +2123,7 @@
         <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2128,7 +2133,7 @@
         <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>142</v>
@@ -2141,7 +2146,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>142</v>
@@ -2158,7 +2163,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>142</v>
@@ -2171,7 +2176,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>142</v>
@@ -2184,7 +2189,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>142</v>
@@ -2197,7 +2202,7 @@
         <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>142</v>
@@ -2212,7 +2217,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>142</v>
@@ -2225,7 +2230,7 @@
         <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>142</v>
@@ -2238,7 +2243,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>142</v>
@@ -2251,7 +2256,7 @@
         <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>142</v>
@@ -2264,7 +2269,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>142</v>
@@ -2323,7 +2328,7 @@
         <v>133</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>134</v>
@@ -3391,67 +3396,82 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B5"/>
+  <autoFilter ref="A1:C5"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3467,8 +3487,9 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -3478,13 +3499,13 @@
         <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>68</v>
@@ -3496,10 +3517,10 @@
         <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>66</v>
@@ -3514,10 +3535,10 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>66</v>
@@ -3528,10 +3549,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Update on 20250806 part 7
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="159">
   <si>
     <t>东方卫视</t>
   </si>
@@ -2132,27 +2132,29 @@
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Update on 20250813 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$J$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$I$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="160">
   <si>
     <t>东方卫视</t>
   </si>
@@ -570,6 +570,10 @@
   </si>
   <si>
     <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极直播</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2122,10 +2126,10 @@
       <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -2327,7 +2331,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2340,12 +2344,12 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="9" width="9.125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
@@ -2370,12 +2374,15 @@
       <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>137</v>
       </c>
@@ -2394,13 +2401,14 @@
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2423,8 +2431,11 @@
         <v>39</v>
       </c>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2447,8 +2458,11 @@
         <v>39</v>
       </c>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2469,9 +2483,10 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I5" s="5"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2492,9 +2507,12 @@
         <v>39</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2509,9 +2527,10 @@
       <c r="H7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I7" s="5"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>145</v>
       </c>
@@ -2536,9 +2555,12 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2563,8 +2585,11 @@
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2587,8 +2612,9 @@
         <v>39</v>
       </c>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2613,8 +2639,11 @@
       <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2635,8 +2664,9 @@
         <v>39</v>
       </c>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2657,8 +2687,11 @@
         <v>39</v>
       </c>
       <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2683,8 +2716,11 @@
       <c r="H14" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2703,8 +2739,9 @@
       <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2727,8 +2764,11 @@
         <v>39</v>
       </c>
       <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2753,8 +2793,11 @@
       <c r="H17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2779,8 +2822,11 @@
       <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2805,8 +2851,11 @@
       <c r="H19" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2827,8 +2876,11 @@
         <v>39</v>
       </c>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -2853,8 +2905,11 @@
       <c r="H21" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2879,8 +2934,11 @@
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2905,8 +2963,11 @@
       <c r="H23" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
@@ -2925,9 +2986,10 @@
       <c r="F24" s="5"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I24" s="10"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -2950,8 +3012,11 @@
         <v>39</v>
       </c>
       <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -2966,9 +3031,10 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="16"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I26" s="10"/>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2991,8 +3057,9 @@
         <v>39</v>
       </c>
       <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -3015,8 +3082,9 @@
         <v>39</v>
       </c>
       <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
@@ -3031,9 +3099,10 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="16"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I29" s="10"/>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -3058,8 +3127,11 @@
       <c r="H30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -3078,8 +3150,9 @@
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3096,9 +3169,10 @@
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="16"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I32" s="10"/>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3115,9 +3189,10 @@
       <c r="F33" s="5"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="16"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I33" s="10"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3140,8 +3215,9 @@
         <v>39</v>
       </c>
       <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -3164,8 +3240,9 @@
         <v>39</v>
       </c>
       <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -3190,8 +3267,11 @@
       <c r="H36" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -3212,8 +3292,11 @@
         <v>39</v>
       </c>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -3236,8 +3319,11 @@
         <v>39</v>
       </c>
       <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I38" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -3258,8 +3344,11 @@
         <v>39</v>
       </c>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -3278,9 +3367,10 @@
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="I40" s="16"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I40" s="10"/>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -3303,8 +3393,9 @@
         <v>39</v>
       </c>
       <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -3319,9 +3410,10 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-      <c r="I42" s="16"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I42" s="10"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -3344,8 +3436,11 @@
         <v>39</v>
       </c>
       <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -3364,9 +3459,10 @@
       <c r="F44" s="5"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
-      <c r="I44" s="16"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I44" s="10"/>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -3389,8 +3485,9 @@
         <v>39</v>
       </c>
       <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -3413,9 +3510,12 @@
         <v>39</v>
       </c>
       <c r="H46" s="5"/>
+      <c r="I46" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H46"/>
+  <autoFilter ref="A1:I46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250817 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -15,19 +15,19 @@
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$J$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$I$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$G$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$E$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="154">
   <si>
     <t>东方卫视</t>
   </si>
@@ -238,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>江西组播源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -395,10 +391,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CGTN英语</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -485,10 +477,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>高清,标清</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -510,24 +498,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>百视通</t>
-  </si>
-  <si>
-    <t>NPTV</t>
-  </si>
-  <si>
-    <t>GPTV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>东方卫视</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NPTV,咪咕源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>直播源1</t>
   </si>
   <si>
@@ -545,7 +519,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直播源3</t>
+    <t>上海移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方购物一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪咕代理源</t>
+  </si>
+  <si>
+    <t>咪咕代理源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -553,27 +546,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上海移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东方购物一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>极直播</t>
+    <t>极直播PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极直播PHP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -682,19 +659,15 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -706,12 +679,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1022,404 +993,397 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="11" customWidth="1"/>
     <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>153</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F1" s="14"/>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>144</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1427,62 +1391,56 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>144</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="1"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="1"/>
@@ -1490,23 +1448,21 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="1"/>
@@ -1514,10 +1470,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="1"/>
@@ -1525,23 +1481,23 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="1"/>
@@ -1549,10 +1505,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="1"/>
@@ -1560,49 +1516,43 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="1"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="1"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="1"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1618,7 +1568,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1628,55 +1578,41 @@
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
@@ -1688,25 +1624,20 @@
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="I2" s="8"/>
+      <c r="J2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -1718,27 +1649,20 @@
       <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -1748,16 +1672,11 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1772,20 +1691,13 @@
       <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="G5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
@@ -1802,18 +1714,11 @@
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
@@ -1825,19 +1730,14 @@
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
@@ -1849,19 +1749,14 @@
       <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -1873,19 +1768,14 @@
       <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>
@@ -1897,19 +1787,14 @@
       <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
@@ -1921,18 +1806,13 @@
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J11"/>
+  <autoFilter ref="A1:G11"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1941,43 +1821,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1985,20 +1861,17 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -2006,20 +1879,17 @@
         <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
@@ -2027,50 +1897,43 @@
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -2078,16 +1941,13 @@
         <v>62</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2095,16 +1955,13 @@
         <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
@@ -2112,14 +1969,11 @@
         <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>65</v>
       </c>
@@ -2127,25 +1981,23 @@
         <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2153,12 +2005,11 @@
         <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2166,14 +2017,11 @@
         <v>62</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2181,149 +2029,110 @@
         <v>62</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E24"/>
+  <autoFilter ref="A1:D24"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2331,7 +2140,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2342,49 +2151,43 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="10" width="9.125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
@@ -2396,19 +2199,15 @@
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H2" s="13"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2427,15 +2226,15 @@
       <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2457,12 +2256,8 @@
       <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2478,15 +2273,13 @@
       <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>40</v>
+      <c r="F5" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2500,19 +2293,15 @@
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>39</v>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2522,17 +2311,15 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -2552,15 +2339,9 @@
       <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2582,14 +2363,8 @@
       <c r="G9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2605,16 +2380,12 @@
       <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2636,14 +2407,8 @@
       <c r="G11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2657,16 +2422,12 @@
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2683,15 +2444,11 @@
       <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2710,17 +2467,11 @@
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2735,13 +2486,9 @@
       <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2760,15 +2507,11 @@
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2784,20 +2527,14 @@
       <c r="E17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2819,14 +2556,8 @@
       <c r="G18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2845,17 +2576,11 @@
       <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2875,12 +2600,8 @@
       <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -2896,20 +2617,14 @@
       <c r="E21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2931,14 +2646,8 @@
       <c r="G22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2960,16 +2669,10 @@
       <c r="G23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>41</v>
@@ -2983,13 +2686,11 @@
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -3008,15 +2709,11 @@
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -3030,11 +2727,9 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -3053,13 +2748,9 @@
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -3078,15 +2769,11 @@
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>41</v>
@@ -3098,11 +2785,9 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -3121,17 +2806,11 @@
       <c r="F30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -3145,14 +2824,10 @@
         <v>40</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3164,15 +2839,11 @@
         <v>40</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="16"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3186,13 +2857,11 @@
       <c r="E33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3211,13 +2880,9 @@
       <c r="F34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -3236,13 +2901,9 @@
       <c r="F35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -3258,20 +2919,14 @@
       <c r="E36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>40</v>
+      <c r="F36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -3291,12 +2946,8 @@
       <c r="G37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -3312,18 +2963,14 @@
       <c r="E38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -3340,15 +2987,11 @@
       <c r="F39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -3362,15 +3005,11 @@
         <v>40</v>
       </c>
       <c r="E40" s="10"/>
-      <c r="F40" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -3389,31 +3028,27 @@
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -3432,15 +3067,11 @@
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -3456,13 +3087,11 @@
       <c r="E44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="F44" s="10"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -3478,16 +3107,12 @@
       <c r="E45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="F45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -3509,13 +3134,9 @@
       <c r="G46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I46"/>
+  <autoFilter ref="A1:G46"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3539,63 +3160,63 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3608,86 +3229,72 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D4"/>
+  <autoFilter ref="A1:C4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20250818 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="154">
   <si>
     <t>东方卫视</t>
   </si>
@@ -2933,7 +2933,9 @@
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250824 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$F$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$C$4</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -559,6 +559,10 @@
   </si>
   <si>
     <t>海南移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2253,7 +2257,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2314,7 +2320,9 @@
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="13"/>
@@ -3228,7 +3236,9 @@
         <v>40</v>
       </c>
       <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="F40" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="13"/>
@@ -3385,7 +3395,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3394,11 +3404,12 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
@@ -3408,12 +3419,15 @@
       <c r="C1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>125</v>
       </c>
@@ -3423,12 +3437,15 @@
       <c r="C2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>126</v>
       </c>
@@ -3438,8 +3455,11 @@
       <c r="C3" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D3" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>136</v>
       </c>
@@ -3449,8 +3469,9 @@
       <c r="C4" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -3460,9 +3481,12 @@
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C5"/>
+  <autoFilter ref="A1:D5"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250828 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -2257,9 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3127,8 +3125,8 @@
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>40</v>
+      <c r="C36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Update on 20250902 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -3037,7 +3037,9 @@
       <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250922 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="157">
   <si>
     <t>东方卫视</t>
   </si>
@@ -2442,7 +2442,9 @@
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250923 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -15,19 +15,19 @@
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$F$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="159">
   <si>
     <t>东方卫视</t>
   </si>
@@ -507,62 +507,70 @@
     <t>直播源3</t>
   </si>
   <si>
+    <t>上海移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方购物一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>直播源1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>咪咕代理源</t>
+  </si>
+  <si>
+    <t>咪咕代理源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极直播PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极直播PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海南移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CETV-早期教育</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>直播源2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上海移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东方购物一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源2</t>
+    <t>直播源3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>直播源1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>咪咕代理源</t>
-  </si>
-  <si>
-    <t>咪咕代理源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>极直播PHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>极直播PHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>海南移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1024,13 +1032,13 @@
         <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="1" t="s">
@@ -1043,19 +1051,19 @@
         <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="1" t="s">
@@ -1067,19 +1075,19 @@
         <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1" t="s">
@@ -1091,19 +1099,19 @@
         <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -1111,19 +1119,19 @@
         <v>117</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -1131,10 +1139,10 @@
         <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1145,10 +1153,10 @@
         <v>119</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1159,19 +1167,19 @@
         <v>98</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -1182,13 +1190,13 @@
         <v>124</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -1197,19 +1205,19 @@
         <v>99</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1217,19 +1225,19 @@
         <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1237,19 +1245,19 @@
         <v>101</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -1257,19 +1265,19 @@
         <v>102</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -1277,19 +1285,19 @@
         <v>103</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1297,19 +1305,19 @@
         <v>104</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -1317,19 +1325,19 @@
         <v>105</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -1337,19 +1345,19 @@
         <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -1357,19 +1365,19 @@
         <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1377,19 +1385,19 @@
         <v>108</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1397,13 +1405,13 @@
         <v>109</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="5"/>
@@ -1413,17 +1421,17 @@
         <v>120</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -1431,7 +1439,7 @@
         <v>121</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="5"/>
@@ -1464,10 +1472,12 @@
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
       <c r="F25" s="5"/>
@@ -1476,10 +1486,12 @@
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
       <c r="F26" s="5"/>
@@ -1488,10 +1500,12 @@
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="1"/>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
       <c r="F27" s="5"/>
@@ -1500,10 +1514,12 @@
       <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="1"/>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
       <c r="F28" s="5"/>
@@ -1512,10 +1528,12 @@
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
       <c r="F29" s="5"/>
@@ -1524,10 +1542,12 @@
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1"/>
       <c r="D30" s="5"/>
       <c r="E30" s="1"/>
       <c r="F30" s="5"/>
@@ -1536,10 +1556,12 @@
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="1"/>
       <c r="F31" s="5"/>
@@ -1548,10 +1570,12 @@
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="1"/>
       <c r="F32" s="5"/>
@@ -1560,10 +1584,12 @@
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="1"/>
       <c r="F33" s="5"/>
@@ -1572,10 +1598,12 @@
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
       <c r="F34" s="5"/>
@@ -1584,10 +1612,12 @@
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="1"/>
       <c r="F35" s="5"/>
@@ -1597,9 +1627,9 @@
         <v>86</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="5"/>
       <c r="E36" s="1"/>
       <c r="F36" s="5"/>
@@ -1609,9 +1639,9 @@
         <v>87</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="5"/>
       <c r="E37" s="1"/>
       <c r="F37" s="5"/>
@@ -1621,9 +1651,9 @@
         <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C38" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="5"/>
       <c r="E38" s="1"/>
       <c r="F38" s="5"/>
@@ -1650,13 +1680,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -1678,16 +1708,16 @@
         <v>62</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>124</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>66</v>
@@ -1793,32 +1823,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>111</v>
+      <c r="A6" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="1"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
@@ -1826,7 +1848,9 @@
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
@@ -1840,7 +1864,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
@@ -1862,7 +1886,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -1884,7 +1908,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>
@@ -1906,7 +1930,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
@@ -1926,8 +1950,30 @@
       </c>
       <c r="H11" s="1"/>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H11"/>
+  <autoFilter ref="A1:H12"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1976,10 +2022,10 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
@@ -1994,10 +2040,10 @@
         <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="1" t="s">
@@ -2012,7 +2058,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>89</v>
@@ -2039,10 +2085,10 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>89</v>
@@ -2056,10 +2102,10 @@
         <v>62</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -2070,7 +2116,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>89</v>
@@ -2084,7 +2130,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2102,13 +2148,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2120,7 +2166,7 @@
         <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2132,7 +2178,7 @@
         <v>62</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2144,7 +2190,7 @@
         <v>62</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>66</v>
@@ -2155,7 +2201,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2165,7 +2211,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2175,7 +2221,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="5"/>
@@ -2185,7 +2231,7 @@
         <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2203,7 +2249,7 @@
         <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="5"/>
@@ -2213,7 +2259,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="5"/>
@@ -2223,7 +2269,7 @@
         <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="5"/>
@@ -2233,7 +2279,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2285,19 +2331,19 @@
         <v>130</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>131</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>67</v>
@@ -3416,13 +3462,13 @@
         <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>67</v>
@@ -3434,13 +3480,13 @@
         <v>125</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="1" t="s">
@@ -3452,13 +3498,13 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -3469,7 +3515,7 @@
         <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -3478,13 +3524,13 @@
         <v>127</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3497,72 +3543,89 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>148</v>
+      <c r="B2" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>148</v>
+      <c r="B3" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F3" s="4"/>
+      <c r="G3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>148</v>
+      <c r="B4" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C4"/>
+  <autoFilter ref="A1:D4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20250924 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="159">
   <si>
     <t>东方卫视</t>
   </si>
@@ -3445,7 +3445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3517,7 +3519,9 @@
       <c r="C4" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250924 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="159">
   <si>
     <t>东方卫视</t>
   </si>
@@ -3445,9 +3445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3519,9 +3517,7 @@
       <c r="C4" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Update on 20250925 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -13,6 +13,7 @@
     <sheet name="卫视" sheetId="1" r:id="rId4"/>
     <sheet name="体育" sheetId="5" r:id="rId5"/>
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
+    <sheet name="其他备注" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$12</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="166">
   <si>
     <t>东方卫视</t>
   </si>
@@ -571,6 +572,34 @@
   </si>
   <si>
     <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>劲爆体育</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>睛彩青少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咪视界</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCTV-5+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥羊代理源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代理源失效,可平替观赛频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3629,4 +3658,79 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20251008 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">其他备注!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="170">
   <si>
     <t>东方卫视</t>
   </si>
@@ -591,10 +592,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>当前源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>肥羊代理源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,6 +605,18 @@
   </si>
   <si>
     <t>冰茶TV助手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不知名PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1050,7 +1059,7 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.125" style="11" customWidth="1"/>
@@ -1223,19 +1232,21 @@
       <c r="A9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
@@ -3670,54 +3681,61 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>159</v>
       </c>
@@ -3725,29 +3743,32 @@
         <v>146</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20251009 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$F$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="172">
   <si>
     <t>东方卫视</t>
   </si>
@@ -617,6 +617,14 @@
   </si>
   <si>
     <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视新闻PHP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1051,23 +1059,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
@@ -1086,13 +1096,16 @@
       <c r="F1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>95</v>
       </c>
@@ -1109,14 +1122,17 @@
         <v>146</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1133,14 +1149,17 @@
         <v>146</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -1156,11 +1175,12 @@
       <c r="E4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>117</v>
       </c>
@@ -1177,10 +1197,13 @@
         <v>146</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
@@ -1193,8 +1216,9 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
@@ -1207,8 +1231,9 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -1224,16 +1249,17 @@
       <c r="E8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>167</v>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>124</v>
@@ -1241,14 +1267,15 @@
       <c r="D9" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
@@ -1264,11 +1291,12 @@
       <c r="E10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
@@ -1285,10 +1313,13 @@
         <v>146</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
@@ -1304,11 +1335,12 @@
       <c r="E12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -1325,10 +1357,13 @@
         <v>146</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -1345,10 +1380,13 @@
         <v>146</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
@@ -1364,11 +1402,12 @@
       <c r="E15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
@@ -1385,10 +1424,13 @@
         <v>146</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
@@ -1405,10 +1447,13 @@
         <v>146</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -1424,11 +1469,12 @@
       <c r="E18" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -1444,11 +1490,12 @@
       <c r="E19" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>109</v>
       </c>
@@ -1463,8 +1510,9 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -1474,27 +1522,35 @@
       <c r="C21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -1503,8 +1559,9 @@
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1515,8 +1572,9 @@
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -1529,8 +1587,9 @@
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -1543,8 +1602,9 @@
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -1557,8 +1617,9 @@
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
       <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
@@ -1571,8 +1632,9 @@
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -1585,8 +1647,9 @@
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
       <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
@@ -1599,8 +1662,9 @@
       <c r="D30" s="5"/>
       <c r="E30" s="1"/>
       <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
@@ -1613,8 +1677,9 @@
       <c r="D31" s="5"/>
       <c r="E31" s="1"/>
       <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -1627,8 +1692,9 @@
       <c r="D32" s="5"/>
       <c r="E32" s="1"/>
       <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1641,8 +1707,9 @@
       <c r="D33" s="5"/>
       <c r="E33" s="1"/>
       <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
@@ -1655,8 +1722,9 @@
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
@@ -1669,8 +1737,9 @@
       <c r="D35" s="5"/>
       <c r="E35" s="1"/>
       <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
@@ -1681,8 +1750,9 @@
       <c r="D36" s="5"/>
       <c r="E36" s="1"/>
       <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>87</v>
       </c>
@@ -1693,8 +1763,9 @@
       <c r="D37" s="5"/>
       <c r="E37" s="1"/>
       <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -1705,8 +1776,9 @@
       <c r="D38" s="5"/>
       <c r="E38" s="1"/>
       <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1717,9 +1789,10 @@
       <c r="D39" s="5"/>
       <c r="E39" s="1"/>
       <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F39"/>
+  <autoFilter ref="A1:G39"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20251014 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -13,15 +13,13 @@
     <sheet name="卫视" sheetId="1" r:id="rId4"/>
     <sheet name="体育" sheetId="5" r:id="rId5"/>
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
-    <sheet name="其他备注" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">其他备注!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$F$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">央视!$A$1:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="164">
   <si>
     <t>东方卫视</t>
   </si>
@@ -540,6 +538,50 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>直播源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海南移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CETV-早期教育</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视新闻PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北广电PHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱上海</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播源6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>直播源4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -548,87 +590,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直播源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>海南移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CETV-早期教育</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>劲爆体育</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>睛彩青少</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>咪视界</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCTV-5+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>肥羊代理源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代理源失效,可平替观赛频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备用源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冰茶TV助手</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不知名PHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播源2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>央视新闻PHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>湖北广电PHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>爱上海</t>
+    <t>抖音直播间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1063,7 +1025,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1071,15 +1033,16 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="15" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
@@ -1090,21 +1053,24 @@
         <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F1" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>95</v>
       </c>
@@ -1115,20 +1081,21 @@
         <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1139,20 +1106,23 @@
         <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -1163,14 +1133,15 @@
         <v>124</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>117</v>
       </c>
@@ -1181,16 +1152,17 @@
         <v>124</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
@@ -1203,8 +1175,9 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
@@ -1217,8 +1190,9 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -1229,34 +1203,34 @@
         <v>124</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
@@ -1267,14 +1241,17 @@
         <v>124</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
@@ -1285,16 +1262,19 @@
         <v>124</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
@@ -1305,14 +1285,15 @@
         <v>124</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -1323,16 +1304,17 @@
         <v>124</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -1343,16 +1325,17 @@
         <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
@@ -1363,14 +1346,15 @@
         <v>124</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
@@ -1381,16 +1365,17 @@
         <v>124</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
@@ -1401,16 +1386,19 @@
         <v>124</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -1421,14 +1409,15 @@
         <v>124</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -1439,14 +1428,15 @@
         <v>124</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>109</v>
       </c>
@@ -1457,12 +1447,13 @@
         <v>124</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -1473,16 +1464,17 @@
         <v>124</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -1490,23 +1482,25 @@
         <v>142</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1515,10 +1509,11 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -1529,10 +1524,11 @@
         <v>66</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -1543,10 +1539,11 @@
         <v>66</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -1557,10 +1554,11 @@
         <v>66</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
@@ -1571,10 +1569,11 @@
         <v>66</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -1585,10 +1584,11 @@
         <v>66</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
@@ -1599,10 +1599,11 @@
         <v>66</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
@@ -1613,10 +1614,11 @@
         <v>66</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -1627,10 +1629,11 @@
         <v>66</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1641,10 +1644,11 @@
         <v>66</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
@@ -1655,10 +1659,11 @@
         <v>66</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
@@ -1669,10 +1674,11 @@
         <v>66</v>
       </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
@@ -1681,10 +1687,11 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>87</v>
       </c>
@@ -1693,10 +1700,11 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -1705,10 +1713,11 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="1"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1717,11 +1726,12 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
+      <c r="G39" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F39"/>
+  <autoFilter ref="A1:G39"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1764,7 +1774,7 @@
         <v>124</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>147</v>
@@ -1874,7 +1884,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
@@ -2121,15 +2131,13 @@
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
@@ -2197,7 +2205,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>62</v>
@@ -2300,7 +2308,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>146</v>
@@ -2366,7 +2374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2400,7 +2408,7 @@
         <v>131</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>147</v>
@@ -3533,7 +3541,7 @@
         <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>67</v>
@@ -3551,7 +3559,7 @@
         <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="1" t="s">
@@ -3569,7 +3577,7 @@
         <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -3580,7 +3588,7 @@
         <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -3595,7 +3603,7 @@
         <v>124</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3626,13 +3634,13 @@
         <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>67</v>
@@ -3694,100 +3702,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:E4"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20251021 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
+++ b/直播源汇总文档/其他文档/常看频道直播源统计.xlsx
@@ -15,7 +15,7 @@
     <sheet name="娱乐" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CETV和CGTN!$A$1:$I$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">卫视!$A$1:$H$46</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="165">
   <si>
     <t>东方卫视</t>
   </si>
@@ -591,6 +591,10 @@
   </si>
   <si>
     <t>抖音直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广西电视台官网</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1740,7 +1744,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1753,11 +1757,12 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -1782,12 +1787,15 @@
       <c r="H1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -1810,12 +1818,15 @@
       <c r="H2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1838,12 +1849,15 @@
       <c r="H3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>137</v>
       </c>
@@ -1856,9 +1870,10 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I4" s="1"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -1881,8 +1896,11 @@
       <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>153</v>
       </c>
@@ -1897,8 +1915,9 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>111</v>
       </c>
@@ -1921,8 +1940,9 @@
         <v>40</v>
       </c>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>112</v>
       </c>
@@ -1943,8 +1963,9 @@
         <v>40</v>
       </c>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>113</v>
       </c>
@@ -1965,8 +1986,9 @@
         <v>40</v>
       </c>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>114</v>
       </c>
@@ -1987,8 +2009,9 @@
         <v>40</v>
       </c>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>115</v>
       </c>
@@ -2009,8 +2032,9 @@
         <v>40</v>
       </c>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>116</v>
       </c>
@@ -2031,9 +2055,10 @@
         <v>40</v>
       </c>
       <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12"/>
+  <autoFilter ref="A1:I12"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>